<commit_message>
Updated app.py and templates
</commit_message>
<xml_diff>
--- a/static/combined_service_centers.xlsx
+++ b/static/combined_service_centers.xlsx
@@ -438,10 +438,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>17.24042</v>
+        <v>17.240421</v>
       </c>
       <c r="B5">
-        <v>80.13507199999999</v>
+        <v>80.13507300000001</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Fixed login bug and updated UI
</commit_message>
<xml_diff>
--- a/static/combined_service_centers.xlsx
+++ b/static/combined_service_centers.xlsx
@@ -438,10 +438,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>17.240423</v>
+        <v>17.24011</v>
       </c>
       <c r="B5">
-        <v>80.13507300000001</v>
+        <v>80.13483100000001</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>

</xml_diff>